<commit_message>
Se agregan diagramaas de robustez y de secuencia respectivos a mis CU, se corrigen descripciones de casos de uso y se actualiza plantilla de Casos de Usos
</commit_message>
<xml_diff>
--- a/Plantillas/Iteracion 2/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Iteracion 2/Plantilla de Casos de Uso.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\watwi\Desktop\Archivos - Desarrollo de software\EMA-Desarrollo-de-software-Equipo-2\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\watwi\Desktop\Archivos - Desarrollo de software\EMA-Desarrollo-de-software-Equipo-2\Plantillas\Iteracion 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D9D615-6A81-4E74-8A89-952E894E66E0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="26475" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4530" windowWidth="26475" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="89">
   <si>
     <t>Columna</t>
   </si>
@@ -267,9 +268,6 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>Documento ERS</t>
-  </si>
-  <si>
     <t>Administrar pagos de alumnos</t>
   </si>
   <si>
@@ -288,7 +286,25 @@
     <t>Planificado</t>
   </si>
   <si>
-    <t>01:00 hr</t>
+    <t>Primer parcial</t>
+  </si>
+  <si>
+    <t>05:30 hrs</t>
+  </si>
+  <si>
+    <t>04:30 hrs</t>
+  </si>
+  <si>
+    <t>03:30 hrs</t>
+  </si>
+  <si>
+    <t>04:00 hrs</t>
+  </si>
+  <si>
+    <t>03:30 hr</t>
+  </si>
+  <si>
+    <t>03:00 hrs</t>
   </si>
 </sst>
 </file>
@@ -727,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,13 +809,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>75</v>
@@ -817,13 +833,13 @@
         <v>25</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>75</v>
@@ -841,13 +857,13 @@
         <v>26</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>75</v>
@@ -865,13 +881,13 @@
         <v>45</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>75</v>
@@ -883,19 +899,19 @@
         <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>75</v>
@@ -913,13 +929,13 @@
         <v>46</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>75</v>
@@ -932,19 +948,19 @@
         <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>75</v>
@@ -962,13 +978,13 @@
         <v>48</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>75</v>
@@ -986,13 +1002,13 @@
         <v>49</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>75</v>
@@ -1010,13 +1026,13 @@
         <v>50</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>75</v>
@@ -1034,13 +1050,13 @@
         <v>51</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>75</v>
@@ -1052,19 +1068,19 @@
         <v>37</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="E16" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>75</v>
@@ -1082,13 +1098,13 @@
         <v>52</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>75</v>
@@ -1106,13 +1122,13 @@
         <v>53</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>75</v>
@@ -1130,13 +1146,13 @@
         <v>54</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>75</v>
@@ -1154,13 +1170,13 @@
         <v>55</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>75</v>
@@ -1178,13 +1194,13 @@
         <v>56</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>75</v>
@@ -1202,13 +1218,13 @@
         <v>57</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>75</v>
@@ -1226,13 +1242,13 @@
         <v>58</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>75</v>

</xml_diff>